<commit_message>
F boards routed, various optimisations made
</commit_message>
<xml_diff>
--- a/BGP_F1/BOM.xlsx
+++ b/BGP_F1/BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="74">
   <si>
     <t xml:space="preserve">BUF</t>
   </si>
@@ -35,84 +35,87 @@
     <t xml:space="preserve">499k</t>
   </si>
   <si>
+    <t xml:space="preserve">0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.49k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.99k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3296X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bourns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3296X-1-103LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANTALUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMCP1D104MTRF</t>
+  </si>
+  <si>
     <t xml:space="preserve">0805</t>
   </si>
   <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.49k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.99k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RV1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3296X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bourns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3296X-1-103LF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TANTALUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMCP1D104MTRF</t>
-  </si>
-  <si>
     <t xml:space="preserve">C2</t>
   </si>
   <si>
@@ -146,6 +149,9 @@
     <t xml:space="preserve">TCTP1C106M8R</t>
   </si>
   <si>
+    <t xml:space="preserve">C5</t>
+  </si>
+  <si>
     <t xml:space="preserve">IC</t>
   </si>
   <si>
@@ -192,6 +198,51 @@
   </si>
   <si>
     <t xml:space="preserve">ECH-U1C393GX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMCMA1C226MTRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1H102GX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGF1B-E3/67A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
   </si>
 </sst>
 </file>
@@ -266,9 +317,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -292,18 +347,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -319,10 +377,10 @@
       <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -330,10 +388,10 @@
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -341,10 +399,10 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -352,10 +410,10 @@
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -363,10 +421,10 @@
       <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -374,10 +432,10 @@
       <c r="B7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -385,10 +443,10 @@
       <c r="B8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -396,10 +454,10 @@
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -407,10 +465,10 @@
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -418,10 +476,10 @@
       <c r="B11" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -429,10 +487,10 @@
       <c r="B12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -443,7 +501,7 @@
       <c r="B13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
@@ -463,7 +521,7 @@
       <c r="B14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -478,25 +536,25 @@
       <c r="G14" s="0" t="n">
         <v>0.851</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>4</v>
+      <c r="I14" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>1.34</v>
@@ -504,25 +562,25 @@
       <c r="H15" s="0" t="n">
         <v>0.849</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>35</v>
+      <c r="I15" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>1.34</v>
@@ -530,25 +588,25 @@
       <c r="H16" s="0" t="n">
         <v>0.849</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>35</v>
+      <c r="I16" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.823</v>
@@ -556,245 +614,584 @@
       <c r="H17" s="0" t="n">
         <v>0.679</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>4</v>
+      <c r="I17" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="B18" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.679</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="B19" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="D19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>1.13</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <v>0.955</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B22" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>4</v>
+      <c r="I22" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>4</v>
+      <c r="I25" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="I28" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="D29" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>0.755</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>0.546</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>0.248</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>4</v>
+      <c r="I29" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="G30" s="0" t="n">
-        <v>1.18</v>
+        <v>0.37</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>0.671</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>35</v>
+        <v>0.248</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="E32" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>0.679</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <v>0.823</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>0.679</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="E33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="B34" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="D34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="0" t="n">
         <v>1.13</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H34" s="0" t="n">
+        <v>0.955</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0.796</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="0"/>
+      <c r="E53" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.497</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>0.955</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="H55" s="0" t="n">
         <v>0.955</v>
       </c>
     </row>
@@ -817,7 +1214,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I3:I12 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>